<commit_message>
Chore: Update README.md file
</commit_message>
<xml_diff>
--- a/realestatelistings.xlsx
+++ b/realestatelistings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kwesi\OneDrive\Robots\Robot4_RealEstateScrpaing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{ACBE29EC-55AD-4128-8984-3FB0822F6271}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D909230B-7C04-400C-9426-FFCE78D132DA}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{ACBE29EC-55AD-4128-8984-3FB0822F6271}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{05E35BCA-C04C-463D-838B-FB6AD3D51AAE}"/>
   <bookViews>
     <workbookView xWindow="930" yWindow="780" windowWidth="18000" windowHeight="9480" xr2:uid="{9FEC4217-1201-4D0D-9EB0-CBE3004B3718}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="228">
   <si>
     <t>Pricing</t>
   </si>
@@ -51,12 +51,6 @@
     <t>223 m²</t>
   </si>
   <si>
-    <t>90 m²</t>
-  </si>
-  <si>
-    <t>65 m²</t>
-  </si>
-  <si>
     <t>75 m²</t>
   </si>
   <si>
@@ -78,9 +72,6 @@
     <t>R 1 650 000</t>
   </si>
   <si>
-    <t>R 1 800 000</t>
-  </si>
-  <si>
     <t>R 2 100 000</t>
   </si>
   <si>
@@ -114,9 +105,6 @@
     <t>R 3 800 000</t>
   </si>
   <si>
-    <t>R 4 500 000</t>
-  </si>
-  <si>
     <t>49 m²</t>
   </si>
   <si>
@@ -129,408 +117,30 @@
     <t>70 m²</t>
   </si>
   <si>
-    <t>124 m²</t>
-  </si>
-  <si>
-    <t>727 m²</t>
-  </si>
-  <si>
-    <t>55 m²</t>
-  </si>
-  <si>
-    <t>657 m²</t>
-  </si>
-  <si>
-    <t>1 130 m²</t>
-  </si>
-  <si>
     <t>175 m²</t>
   </si>
   <si>
-    <t>POA</t>
-  </si>
-  <si>
     <t>125 m²</t>
   </si>
   <si>
-    <t>Mouille Point</t>
-  </si>
-  <si>
-    <t>R 1 075 000</t>
-  </si>
-  <si>
-    <t>29 m²</t>
-  </si>
-  <si>
     <t>Wynberg</t>
   </si>
   <si>
-    <t>Heathfield</t>
-  </si>
-  <si>
-    <t>77 m²</t>
-  </si>
-  <si>
-    <t>Kenilworth</t>
-  </si>
-  <si>
-    <t>Westlake</t>
-  </si>
-  <si>
-    <t>R 1 295 000</t>
-  </si>
-  <si>
-    <t>Woodstock</t>
-  </si>
-  <si>
-    <t>60 m²</t>
-  </si>
-  <si>
-    <t>58 m²</t>
-  </si>
-  <si>
-    <t>Claremont Upper</t>
-  </si>
-  <si>
-    <t>R 1 299 000</t>
-  </si>
-  <si>
-    <t>161 m²</t>
-  </si>
-  <si>
-    <t>Costa Da Gama</t>
-  </si>
-  <si>
-    <t>R 1 350 000</t>
-  </si>
-  <si>
-    <t>40 m²</t>
-  </si>
-  <si>
-    <t>Observatory</t>
-  </si>
-  <si>
-    <t>50 m²</t>
-  </si>
-  <si>
-    <t>R 1 385 000</t>
-  </si>
-  <si>
-    <t>54 m²</t>
-  </si>
-  <si>
-    <t>Newlands</t>
-  </si>
-  <si>
-    <t>64 m²</t>
-  </si>
-  <si>
-    <t>R 1 750 000</t>
-  </si>
-  <si>
-    <t>66 m²</t>
-  </si>
-  <si>
-    <t>Fresnaye</t>
-  </si>
-  <si>
-    <t>R 1 845 000</t>
-  </si>
-  <si>
-    <t>Muizenberg</t>
-  </si>
-  <si>
-    <t>R 1 850 000</t>
-  </si>
-  <si>
-    <t>Zonnebloem</t>
-  </si>
-  <si>
-    <t>R 1 875 000</t>
-  </si>
-  <si>
-    <t>204 m²</t>
-  </si>
-  <si>
-    <t>R 1 895 000</t>
-  </si>
-  <si>
-    <t>590 m²</t>
-  </si>
-  <si>
-    <t>Retreat</t>
-  </si>
-  <si>
-    <t>R 1 899 000</t>
-  </si>
-  <si>
-    <t>53 m²</t>
-  </si>
-  <si>
-    <t>R 1 907 000</t>
-  </si>
-  <si>
     <t>Cape Town City Centre</t>
   </si>
   <si>
-    <t>R 1 950 000</t>
-  </si>
-  <si>
     <t>Sea Point</t>
   </si>
   <si>
-    <t>R 1 995 000</t>
-  </si>
-  <si>
-    <t>535 m²</t>
-  </si>
-  <si>
-    <t>Athlone</t>
-  </si>
-  <si>
-    <t>85 m²</t>
-  </si>
-  <si>
-    <t>R 10 900 000</t>
-  </si>
-  <si>
-    <t>980 m²</t>
-  </si>
-  <si>
-    <t>R 11 000 000</t>
-  </si>
-  <si>
-    <t>1 380 m²</t>
-  </si>
-  <si>
-    <t>Capricorn</t>
-  </si>
-  <si>
-    <t>R 11 750 000</t>
-  </si>
-  <si>
-    <t>427 m²</t>
-  </si>
-  <si>
-    <t>Foreshore</t>
-  </si>
-  <si>
-    <t>R 13 450 000</t>
-  </si>
-  <si>
-    <t>694 m²</t>
-  </si>
-  <si>
-    <t>Camps Bay</t>
-  </si>
-  <si>
-    <t>R 14 900 000</t>
-  </si>
-  <si>
-    <t>425 m²</t>
-  </si>
-  <si>
-    <t>Green Point</t>
-  </si>
-  <si>
-    <t>R 14 950 000</t>
-  </si>
-  <si>
-    <t>2 312 m²</t>
-  </si>
-  <si>
-    <t>92 m²</t>
-  </si>
-  <si>
-    <t>Bergvliet</t>
-  </si>
-  <si>
-    <t>R 2 175 000</t>
-  </si>
-  <si>
-    <t>45 m²</t>
-  </si>
-  <si>
-    <t>290 m²</t>
-  </si>
-  <si>
-    <t>R 2 300 000</t>
-  </si>
-  <si>
-    <t>56 m²</t>
-  </si>
-  <si>
-    <t>R 2 375 000</t>
-  </si>
-  <si>
-    <t>306 m²</t>
-  </si>
-  <si>
-    <t>Lakeside</t>
-  </si>
-  <si>
-    <t>R 2 465 000</t>
-  </si>
-  <si>
-    <t>560 m²</t>
-  </si>
-  <si>
-    <t>Marina Da Gama</t>
-  </si>
-  <si>
-    <t>R 2 480 000</t>
-  </si>
-  <si>
-    <t>86 m²</t>
-  </si>
-  <si>
-    <t>Wynberg Upper</t>
-  </si>
-  <si>
-    <t>R 2 495 000</t>
-  </si>
-  <si>
-    <t>497 m²</t>
-  </si>
-  <si>
-    <t>Crawford</t>
-  </si>
-  <si>
-    <t>63 m²</t>
-  </si>
-  <si>
-    <t>833 m²</t>
-  </si>
-  <si>
-    <t>Kirstenhof</t>
-  </si>
-  <si>
-    <t>R 2 750 000</t>
-  </si>
-  <si>
-    <t>De Waterkant</t>
-  </si>
-  <si>
-    <t>321 m²</t>
-  </si>
-  <si>
-    <t>Tokai</t>
-  </si>
-  <si>
-    <t>216 m²</t>
-  </si>
-  <si>
-    <t>R 2 995 000</t>
-  </si>
-  <si>
-    <t>67 m²</t>
-  </si>
-  <si>
-    <t>68 m²</t>
-  </si>
-  <si>
-    <t>R 25 000 000</t>
-  </si>
-  <si>
-    <t>4 011 m²</t>
-  </si>
-  <si>
     <t>Constantia</t>
   </si>
   <si>
-    <t>R 25 950 000</t>
-  </si>
-  <si>
-    <t>R 3 120 000</t>
-  </si>
-  <si>
-    <t>80 m²</t>
-  </si>
-  <si>
-    <t>R 3 150 000</t>
-  </si>
-  <si>
-    <t>652 m²</t>
-  </si>
-  <si>
-    <t>310 m²</t>
-  </si>
-  <si>
-    <t>R 3 200 000</t>
-  </si>
-  <si>
-    <t>276 m²</t>
-  </si>
-  <si>
     <t>Claremont</t>
   </si>
   <si>
-    <t>R 3 250 000</t>
-  </si>
-  <si>
-    <t>720 m²</t>
-  </si>
-  <si>
-    <t>Lansdowne</t>
-  </si>
-  <si>
-    <t>R 3 599 990</t>
-  </si>
-  <si>
-    <t>Bantry Bay</t>
-  </si>
-  <si>
-    <t>R 3 700 000</t>
-  </si>
-  <si>
-    <t>544 m²</t>
-  </si>
-  <si>
-    <t>181 m²</t>
-  </si>
-  <si>
-    <t>R 3 950 000</t>
-  </si>
-  <si>
-    <t>280 m²</t>
-  </si>
-  <si>
     <t>Vredehoek</t>
   </si>
   <si>
-    <t>802 m²</t>
-  </si>
-  <si>
-    <t>Meadowridge</t>
-  </si>
-  <si>
-    <t>R 38 500 000</t>
-  </si>
-  <si>
-    <t>R 4 000 000</t>
-  </si>
-  <si>
-    <t>140 m²</t>
-  </si>
-  <si>
-    <t>127 m²</t>
-  </si>
-  <si>
-    <t>R 4 695 000</t>
-  </si>
-  <si>
-    <t>563 m²</t>
-  </si>
-  <si>
-    <t>R 4 700 000</t>
-  </si>
-  <si>
-    <t>580 m²</t>
-  </si>
-  <si>
-    <t>R 4 750 000</t>
-  </si>
-  <si>
     <t>R 4 950 000</t>
   </si>
   <si>
@@ -652,6 +262,459 @@
   </si>
   <si>
     <t>76 m²</t>
+  </si>
+  <si>
+    <t>R 1 050 000</t>
+  </si>
+  <si>
+    <t>83 m²</t>
+  </si>
+  <si>
+    <t>Oakdene</t>
+  </si>
+  <si>
+    <t>R 1 090 000</t>
+  </si>
+  <si>
+    <t>Cheltondale</t>
+  </si>
+  <si>
+    <t>R 1 095 000</t>
+  </si>
+  <si>
+    <t>495 m²</t>
+  </si>
+  <si>
+    <t>Malvern</t>
+  </si>
+  <si>
+    <t>Lenasia South</t>
+  </si>
+  <si>
+    <t>Bezuidenhout Valley</t>
+  </si>
+  <si>
+    <t>R 1 180 000</t>
+  </si>
+  <si>
+    <t>13 916 m²</t>
+  </si>
+  <si>
+    <t>Glenvista</t>
+  </si>
+  <si>
+    <t>R 1 220 000</t>
+  </si>
+  <si>
+    <t>36 749 m²</t>
+  </si>
+  <si>
+    <t>991 m²</t>
+  </si>
+  <si>
+    <t>Westdene</t>
+  </si>
+  <si>
+    <t>612 m²</t>
+  </si>
+  <si>
+    <t>Elandspark</t>
+  </si>
+  <si>
+    <t>R 1 360 000</t>
+  </si>
+  <si>
+    <t>344 m²</t>
+  </si>
+  <si>
+    <t>Melville</t>
+  </si>
+  <si>
+    <t>R 1 395 000</t>
+  </si>
+  <si>
+    <t>990 m²</t>
+  </si>
+  <si>
+    <t>Johannesburg Central</t>
+  </si>
+  <si>
+    <t>R 1 400 000</t>
+  </si>
+  <si>
+    <t>1 318 m²</t>
+  </si>
+  <si>
+    <t>Winchester Hills</t>
+  </si>
+  <si>
+    <t>R 1 420 000</t>
+  </si>
+  <si>
+    <t>4 000 m²</t>
+  </si>
+  <si>
+    <t>R 1 449 000</t>
+  </si>
+  <si>
+    <t>Tulisa Park</t>
+  </si>
+  <si>
+    <t>435 m²</t>
+  </si>
+  <si>
+    <t>R 1 500 000</t>
+  </si>
+  <si>
+    <t>743 m²</t>
+  </si>
+  <si>
+    <t>Kensington</t>
+  </si>
+  <si>
+    <t>R 1 585 000</t>
+  </si>
+  <si>
+    <t>59 m²</t>
+  </si>
+  <si>
+    <t>Houghton Estate</t>
+  </si>
+  <si>
+    <t>R 1 599 000</t>
+  </si>
+  <si>
+    <t>99 m²</t>
+  </si>
+  <si>
+    <t>184 m²</t>
+  </si>
+  <si>
+    <t>R 1 599 999</t>
+  </si>
+  <si>
+    <t>1 046 m²</t>
+  </si>
+  <si>
+    <t>Mulbarton</t>
+  </si>
+  <si>
+    <t>73 m²</t>
+  </si>
+  <si>
+    <t>Rosebank</t>
+  </si>
+  <si>
+    <t>R 1 680 000</t>
+  </si>
+  <si>
+    <t>1 147 m²</t>
+  </si>
+  <si>
+    <t>R 1 900 000</t>
+  </si>
+  <si>
+    <t>2 024 m²</t>
+  </si>
+  <si>
+    <t>Lyndhurst</t>
+  </si>
+  <si>
+    <t>955 m²</t>
+  </si>
+  <si>
+    <t>Bruma</t>
+  </si>
+  <si>
+    <t>1 052 m²</t>
+  </si>
+  <si>
+    <t>Ridgeway</t>
+  </si>
+  <si>
+    <t>R 2 299 000</t>
+  </si>
+  <si>
+    <t>1 056 m²</t>
+  </si>
+  <si>
+    <t>1 031 m²</t>
+  </si>
+  <si>
+    <t>Liefde En Vrede</t>
+  </si>
+  <si>
+    <t>R 2 400 000</t>
+  </si>
+  <si>
+    <t>266 m²</t>
+  </si>
+  <si>
+    <t>Roodepoort</t>
+  </si>
+  <si>
+    <t>Parkhurst</t>
+  </si>
+  <si>
+    <t>116 m²</t>
+  </si>
+  <si>
+    <t>Riviera</t>
+  </si>
+  <si>
+    <t>R 2 440 000</t>
+  </si>
+  <si>
+    <t>1 228 m²</t>
+  </si>
+  <si>
+    <t>R 2 499 000</t>
+  </si>
+  <si>
+    <t>1 392 m²</t>
+  </si>
+  <si>
+    <t>R 2 500 000</t>
+  </si>
+  <si>
+    <t>Suideroord</t>
+  </si>
+  <si>
+    <t>170 m²</t>
+  </si>
+  <si>
+    <t>Dunkeld West</t>
+  </si>
+  <si>
+    <t>R 2 575 000</t>
+  </si>
+  <si>
+    <t>246 m²</t>
+  </si>
+  <si>
+    <t>Milpark</t>
+  </si>
+  <si>
+    <t>989 m²</t>
+  </si>
+  <si>
+    <t>996 m²</t>
+  </si>
+  <si>
+    <t>155 m²</t>
+  </si>
+  <si>
+    <t>Killarney</t>
+  </si>
+  <si>
+    <t>993 m²</t>
+  </si>
+  <si>
+    <t>South Kensington</t>
+  </si>
+  <si>
+    <t>496 m²</t>
+  </si>
+  <si>
+    <t>R 250 000</t>
+  </si>
+  <si>
+    <t>Rosettenville</t>
+  </si>
+  <si>
+    <t>R 275 000</t>
+  </si>
+  <si>
+    <t>Berea</t>
+  </si>
+  <si>
+    <t>R 3 400 000</t>
+  </si>
+  <si>
+    <t>Oaklands</t>
+  </si>
+  <si>
+    <t>R 3 750 000</t>
+  </si>
+  <si>
+    <t>5 811 m²</t>
+  </si>
+  <si>
+    <t>Braamfontein Werf</t>
+  </si>
+  <si>
+    <t>1 487 m²</t>
+  </si>
+  <si>
+    <t>Eltonhill</t>
+  </si>
+  <si>
+    <t>R 345 000</t>
+  </si>
+  <si>
+    <t>Hillbrow</t>
+  </si>
+  <si>
+    <t>R 4 400 000</t>
+  </si>
+  <si>
+    <t>Aspen Hills Nature Estate</t>
+  </si>
+  <si>
+    <t>R 480 000</t>
+  </si>
+  <si>
+    <t>R 5 850 000</t>
+  </si>
+  <si>
+    <t>1 496 m²</t>
+  </si>
+  <si>
+    <t>R 550 000</t>
+  </si>
+  <si>
+    <t>88 m²</t>
+  </si>
+  <si>
+    <t>Linmeyer</t>
+  </si>
+  <si>
+    <t>33 m²</t>
+  </si>
+  <si>
+    <t>Ormonde</t>
+  </si>
+  <si>
+    <t>R 585 000</t>
+  </si>
+  <si>
+    <t>17 154 m²</t>
+  </si>
+  <si>
+    <t>Bramley View</t>
+  </si>
+  <si>
+    <t>R 610 000</t>
+  </si>
+  <si>
+    <t>R 650 000</t>
+  </si>
+  <si>
+    <t>Braamfontein</t>
+  </si>
+  <si>
+    <t>R 660 000</t>
+  </si>
+  <si>
+    <t>Meredale</t>
+  </si>
+  <si>
+    <t>R 695 000</t>
+  </si>
+  <si>
+    <t>3 836 m²</t>
+  </si>
+  <si>
+    <t>Kibler Park</t>
+  </si>
+  <si>
+    <t>R 750 000</t>
+  </si>
+  <si>
+    <t>450 m²</t>
+  </si>
+  <si>
+    <t>R 785 000</t>
+  </si>
+  <si>
+    <t>Regents Park</t>
+  </si>
+  <si>
+    <t>R 789 000</t>
+  </si>
+  <si>
+    <t>480 m²</t>
+  </si>
+  <si>
+    <t>R 800 000</t>
+  </si>
+  <si>
+    <t>459 m²</t>
+  </si>
+  <si>
+    <t>R 840 000</t>
+  </si>
+  <si>
+    <t>52 m²</t>
+  </si>
+  <si>
+    <t>R 890 000</t>
+  </si>
+  <si>
+    <t>470 m²</t>
+  </si>
+  <si>
+    <t>Sophiatown</t>
+  </si>
+  <si>
+    <t>R 895 000</t>
+  </si>
+  <si>
+    <t>Upper Houghton</t>
+  </si>
+  <si>
+    <t>R 899 000</t>
+  </si>
+  <si>
+    <t>69 m²</t>
+  </si>
+  <si>
+    <t>R 920 000</t>
+  </si>
+  <si>
+    <t>500 m²</t>
+  </si>
+  <si>
+    <t>R 925 000</t>
+  </si>
+  <si>
+    <t>71 m²</t>
+  </si>
+  <si>
+    <t>Bassonia</t>
+  </si>
+  <si>
+    <t>R 950 000</t>
+  </si>
+  <si>
+    <t>106 m²</t>
+  </si>
+  <si>
+    <t>R 979 000</t>
+  </si>
+  <si>
+    <t>630 m²</t>
+  </si>
+  <si>
+    <t>R 985 000</t>
+  </si>
+  <si>
+    <t>R 988 000</t>
+  </si>
+  <si>
+    <t>141 m²</t>
+  </si>
+  <si>
+    <t>Gresswold</t>
+  </si>
+  <si>
+    <t>R 989 000</t>
+  </si>
+  <si>
+    <t>R 995 000</t>
+  </si>
+  <si>
+    <t>6 279 m²</t>
   </si>
 </sst>
 </file>
@@ -1034,14 +1097,26 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
       <c r="B2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
       <c r="B3">
         <v>2</v>
       </c>
@@ -1049,253 +1124,304 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
       <c r="B4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>1</v>
-      </c>
       <c r="C5">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
       <c r="B6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>83</v>
+      </c>
+      <c r="E6" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
       <c r="B7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>88</v>
+      </c>
+      <c r="E7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>91</v>
+      </c>
+      <c r="E8" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
+      <c r="D11" t="s">
+        <v>97</v>
+      </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>102</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>105</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>109</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>109</v>
       </c>
       <c r="E17" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>111</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="E19" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>83</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>113</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1304,447 +1430,474 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>114</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>116</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
+        <v>117</v>
       </c>
       <c r="E22" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="D23" t="s">
-        <v>63</v>
+        <v>118</v>
       </c>
       <c r="E23" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>119</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="E24" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
+        <v>122</v>
       </c>
       <c r="E25" t="s">
-        <v>46</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>24</v>
+        <v>125</v>
       </c>
       <c r="E26" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="B27">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>5</v>
+        <v>127</v>
       </c>
       <c r="E27" t="s">
-        <v>68</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="B28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>129</v>
       </c>
       <c r="E28" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="E29" t="s">
-        <v>46</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>74</v>
+        <v>131</v>
       </c>
       <c r="E30" t="s">
-        <v>75</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>133</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="D31" t="s">
-        <v>77</v>
+        <v>134</v>
       </c>
       <c r="E31" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>77</v>
+        <v>135</v>
       </c>
       <c r="E32" t="s">
-        <v>49</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>137</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>138</v>
       </c>
       <c r="E33" t="s">
-        <v>79</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>137</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>83</v>
       </c>
       <c r="E34" t="s">
-        <v>79</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>80</v>
+        <v>137</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="E35" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>143</v>
       </c>
       <c r="B36">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C36">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>83</v>
+        <v>144</v>
       </c>
       <c r="E36" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>82</v>
+        <v>145</v>
       </c>
       <c r="B37">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>85</v>
+        <v>146</v>
       </c>
       <c r="E37" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>86</v>
+        <v>147</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
       </c>
       <c r="D38" t="s">
-        <v>87</v>
+        <v>146</v>
       </c>
       <c r="E38" t="s">
-        <v>49</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>147</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
       </c>
       <c r="D39" t="s">
-        <v>89</v>
+        <v>146</v>
       </c>
       <c r="E39" t="s">
-        <v>90</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>91</v>
+        <v>147</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>92</v>
+        <v>149</v>
       </c>
       <c r="E40" t="s">
-        <v>93</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>94</v>
+        <v>151</v>
       </c>
       <c r="B41">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C41">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="D41" t="s">
-        <v>95</v>
+        <v>152</v>
       </c>
       <c r="E41" t="s">
-        <v>96</v>
+        <v>153</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>97</v>
+        <v>17</v>
       </c>
       <c r="B42">
         <v>3</v>
       </c>
       <c r="C42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>98</v>
+        <v>154</v>
       </c>
       <c r="E42" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>100</v>
+        <v>18</v>
       </c>
       <c r="B43">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C43">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="D43" t="s">
-        <v>101</v>
+        <v>155</v>
       </c>
       <c r="E43" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B44">
         <v>2</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>102</v>
+        <v>156</v>
       </c>
       <c r="E44" t="s">
-        <v>103</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>104</v>
+        <v>19</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>105</v>
+        <v>158</v>
       </c>
       <c r="E45" t="s">
-        <v>79</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>30</v>
+        <v>160</v>
       </c>
       <c r="E46" t="s">
-        <v>79</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>18</v>
+        <v>161</v>
       </c>
       <c r="B47">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>106</v>
+        <v>21</v>
       </c>
       <c r="E47" t="s">
-        <v>43</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>107</v>
+        <v>163</v>
       </c>
       <c r="B48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>108</v>
+        <v>6</v>
       </c>
       <c r="E48" t="s">
-        <v>81</v>
+        <v>164</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>109</v>
+        <v>165</v>
       </c>
       <c r="B49">
         <v>3</v>
@@ -1753,15 +1906,15 @@
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="E49" t="s">
-        <v>111</v>
+        <v>166</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>165</v>
       </c>
       <c r="B50">
         <v>3</v>
@@ -1770,83 +1923,83 @@
         <v>2</v>
       </c>
       <c r="D50" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E50" t="s">
-        <v>49</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>112</v>
+        <v>167</v>
       </c>
       <c r="B51">
         <v>3</v>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D51" t="s">
-        <v>113</v>
+        <v>168</v>
       </c>
       <c r="E51" t="s">
-        <v>114</v>
+        <v>169</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>112</v>
+        <v>23</v>
       </c>
       <c r="B52">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C52">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="D52" t="s">
-        <v>113</v>
+        <v>170</v>
       </c>
       <c r="E52" t="s">
-        <v>114</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>115</v>
+        <v>172</v>
       </c>
       <c r="B53">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>116</v>
+        <v>29</v>
       </c>
       <c r="E53" t="s">
-        <v>117</v>
+        <v>173</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>118</v>
+        <v>174</v>
       </c>
       <c r="B54">
         <v>4</v>
       </c>
       <c r="C54">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D54" t="s">
-        <v>119</v>
+        <v>7</v>
       </c>
       <c r="E54" t="s">
-        <v>120</v>
+        <v>175</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>20</v>
+        <v>176</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -1855,303 +2008,321 @@
         <v>1</v>
       </c>
       <c r="D55" t="s">
-        <v>121</v>
+        <v>24</v>
       </c>
       <c r="E55" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>21</v>
+        <v>177</v>
       </c>
       <c r="B56">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C56">
-        <v>2.5</v>
+        <v>6.5</v>
       </c>
       <c r="D56" t="s">
-        <v>122</v>
+        <v>178</v>
       </c>
       <c r="E56" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>124</v>
+        <v>179</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
+      <c r="D57" t="s">
+        <v>180</v>
+      </c>
       <c r="E57" t="s">
-        <v>125</v>
+        <v>181</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>22</v>
+        <v>179</v>
       </c>
       <c r="B58">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>126</v>
+        <v>182</v>
       </c>
       <c r="E58" t="s">
-        <v>127</v>
+        <v>183</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>23</v>
+        <v>184</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>128</v>
+        <v>185</v>
       </c>
       <c r="E59" t="s">
-        <v>79</v>
+        <v>186</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>129</v>
+        <v>187</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
       <c r="D60" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="E60" t="s">
-        <v>99</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>129</v>
+        <v>188</v>
       </c>
       <c r="B61">
         <v>1</v>
       </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
       <c r="D61" t="s">
-        <v>131</v>
+        <v>25</v>
       </c>
       <c r="E61" t="s">
-        <v>81</v>
+        <v>189</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>132</v>
+        <v>190</v>
       </c>
       <c r="B62">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C62">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>133</v>
+        <v>26</v>
       </c>
       <c r="E62" t="s">
-        <v>134</v>
+        <v>191</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>135</v>
+        <v>192</v>
       </c>
       <c r="B63">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C63">
-        <v>4.5</v>
+        <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>9</v>
+        <v>193</v>
       </c>
       <c r="E63" t="s">
-        <v>96</v>
+        <v>194</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>136</v>
+        <v>195</v>
       </c>
       <c r="B64">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D64" t="s">
-        <v>137</v>
+        <v>196</v>
       </c>
       <c r="E64" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>138</v>
+        <v>197</v>
       </c>
       <c r="B65">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C65">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="E65" t="s">
-        <v>114</v>
+        <v>198</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>138</v>
+        <v>199</v>
       </c>
       <c r="B66">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C66">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>139</v>
+        <v>200</v>
       </c>
       <c r="E66" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>138</v>
+        <v>201</v>
       </c>
       <c r="B67">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>140</v>
+        <v>202</v>
       </c>
       <c r="E67" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>141</v>
+        <v>203</v>
       </c>
       <c r="B68">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C68">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="D68" t="s">
-        <v>142</v>
+        <v>204</v>
       </c>
       <c r="E68" t="s">
-        <v>143</v>
+        <v>79</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>144</v>
+        <v>203</v>
       </c>
       <c r="B69">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C69">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D69" t="s">
-        <v>145</v>
+        <v>204</v>
       </c>
       <c r="E69" t="s">
-        <v>146</v>
+        <v>79</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>147</v>
+        <v>205</v>
       </c>
       <c r="B70">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D70" t="s">
-        <v>34</v>
+        <v>206</v>
       </c>
       <c r="E70" t="s">
-        <v>148</v>
+        <v>207</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>149</v>
+        <v>208</v>
       </c>
       <c r="B71">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C71">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D71" t="s">
-        <v>150</v>
+        <v>27</v>
       </c>
       <c r="E71" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>149</v>
+        <v>208</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
       </c>
       <c r="D72" t="s">
-        <v>151</v>
+        <v>122</v>
       </c>
       <c r="E72" t="s">
-        <v>47</v>
+        <v>209</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>26</v>
+        <v>210</v>
       </c>
       <c r="B73">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D73" t="s">
-        <v>77</v>
+        <v>211</v>
       </c>
       <c r="E73" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>152</v>
+        <v>212</v>
       </c>
       <c r="B74">
         <v>3</v>
@@ -2160,46 +2331,49 @@
         <v>1</v>
       </c>
       <c r="D74" t="s">
-        <v>153</v>
+        <v>213</v>
       </c>
       <c r="E74" t="s">
-        <v>154</v>
+        <v>207</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>152</v>
+        <v>214</v>
       </c>
       <c r="B75">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C75">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D75" t="s">
-        <v>155</v>
+        <v>215</v>
       </c>
       <c r="E75" t="s">
-        <v>156</v>
+        <v>216</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>157</v>
+        <v>217</v>
       </c>
       <c r="B76">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C76">
-        <v>3.5</v>
+        <v>2</v>
+      </c>
+      <c r="D76" t="s">
+        <v>218</v>
       </c>
       <c r="E76" t="s">
-        <v>96</v>
+        <v>191</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>158</v>
+        <v>219</v>
       </c>
       <c r="B77">
         <v>3</v>
@@ -2208,18 +2382,18 @@
         <v>2</v>
       </c>
       <c r="D77" t="s">
-        <v>159</v>
+        <v>220</v>
       </c>
       <c r="E77" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>27</v>
+        <v>221</v>
       </c>
       <c r="B78">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -2228,29 +2402,29 @@
         <v>160</v>
       </c>
       <c r="E78" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>161</v>
+        <v>222</v>
       </c>
       <c r="B79">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C79">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D79" t="s">
-        <v>162</v>
+        <v>223</v>
       </c>
       <c r="E79" t="s">
-        <v>58</v>
+        <v>224</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>163</v>
+        <v>225</v>
       </c>
       <c r="B80">
         <v>4</v>
@@ -2259,32 +2433,32 @@
         <v>2</v>
       </c>
       <c r="D80" t="s">
-        <v>164</v>
+        <v>220</v>
       </c>
       <c r="E80" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>165</v>
+        <v>226</v>
       </c>
       <c r="B81">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C81">
         <v>1</v>
       </c>
       <c r="D81" t="s">
-        <v>31</v>
+        <v>227</v>
       </c>
       <c r="E81" t="s">
-        <v>40</v>
+        <v>148</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>166</v>
+        <v>36</v>
       </c>
       <c r="B82">
         <v>4</v>
@@ -2293,15 +2467,15 @@
         <v>3</v>
       </c>
       <c r="D82" t="s">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="E82" t="s">
-        <v>168</v>
+        <v>38</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>166</v>
+        <v>36</v>
       </c>
       <c r="B83">
         <v>4</v>
@@ -2310,15 +2484,15 @@
         <v>3</v>
       </c>
       <c r="D83" t="s">
-        <v>169</v>
+        <v>39</v>
       </c>
       <c r="E83" t="s">
-        <v>170</v>
+        <v>40</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>171</v>
+        <v>41</v>
       </c>
       <c r="B84">
         <v>2</v>
@@ -2327,26 +2501,26 @@
         <v>2</v>
       </c>
       <c r="D84" t="s">
-        <v>172</v>
+        <v>42</v>
       </c>
       <c r="E84" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>173</v>
+        <v>43</v>
       </c>
       <c r="D85" t="s">
-        <v>174</v>
+        <v>44</v>
       </c>
       <c r="E85" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>175</v>
+        <v>45</v>
       </c>
       <c r="B86">
         <v>3</v>
@@ -2355,26 +2529,26 @@
         <v>3</v>
       </c>
       <c r="D86" t="s">
-        <v>176</v>
+        <v>46</v>
       </c>
       <c r="E86" t="s">
-        <v>143</v>
+        <v>34</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>177</v>
+        <v>47</v>
       </c>
       <c r="D87" t="s">
-        <v>178</v>
+        <v>48</v>
       </c>
       <c r="E87" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>179</v>
+        <v>49</v>
       </c>
       <c r="B88">
         <v>4</v>
@@ -2383,15 +2557,15 @@
         <v>2</v>
       </c>
       <c r="D88" t="s">
-        <v>180</v>
+        <v>50</v>
       </c>
       <c r="E88" t="s">
-        <v>181</v>
+        <v>51</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>182</v>
+        <v>52</v>
       </c>
       <c r="B89">
         <v>5</v>
@@ -2400,15 +2574,15 @@
         <v>3</v>
       </c>
       <c r="D89" t="s">
-        <v>183</v>
+        <v>53</v>
       </c>
       <c r="E89" t="s">
-        <v>184</v>
+        <v>54</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>185</v>
+        <v>55</v>
       </c>
       <c r="B90">
         <v>3</v>
@@ -2417,15 +2591,15 @@
         <v>2.5</v>
       </c>
       <c r="D90" t="s">
-        <v>186</v>
+        <v>56</v>
       </c>
       <c r="E90" t="s">
-        <v>187</v>
+        <v>57</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>185</v>
+        <v>55</v>
       </c>
       <c r="B91">
         <v>3</v>
@@ -2434,15 +2608,15 @@
         <v>2.5</v>
       </c>
       <c r="D91" t="s">
-        <v>186</v>
+        <v>56</v>
       </c>
       <c r="E91" t="s">
-        <v>187</v>
+        <v>57</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>188</v>
+        <v>58</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -2451,15 +2625,15 @@
         <v>2</v>
       </c>
       <c r="D92" t="s">
-        <v>189</v>
+        <v>59</v>
       </c>
       <c r="E92" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>190</v>
+        <v>60</v>
       </c>
       <c r="B93">
         <v>4</v>
@@ -2468,26 +2642,26 @@
         <v>4</v>
       </c>
       <c r="D93" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E93" t="s">
-        <v>191</v>
+        <v>61</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>192</v>
+        <v>62</v>
       </c>
       <c r="D94" t="s">
-        <v>193</v>
+        <v>63</v>
       </c>
       <c r="E94" t="s">
-        <v>194</v>
+        <v>64</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>195</v>
+        <v>65</v>
       </c>
       <c r="B95">
         <v>4</v>
@@ -2496,15 +2670,15 @@
         <v>4</v>
       </c>
       <c r="D95" t="s">
-        <v>196</v>
+        <v>66</v>
       </c>
       <c r="E95" t="s">
-        <v>191</v>
+        <v>61</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>197</v>
+        <v>67</v>
       </c>
       <c r="B96">
         <v>3</v>
@@ -2513,15 +2687,15 @@
         <v>3.5</v>
       </c>
       <c r="D96" t="s">
-        <v>198</v>
+        <v>68</v>
       </c>
       <c r="E96" t="s">
-        <v>199</v>
+        <v>69</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>200</v>
+        <v>70</v>
       </c>
       <c r="B97">
         <v>2</v>
@@ -2530,15 +2704,15 @@
         <v>1</v>
       </c>
       <c r="D97" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E97" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>200</v>
+        <v>70</v>
       </c>
       <c r="B98">
         <v>2</v>
@@ -2547,15 +2721,15 @@
         <v>1</v>
       </c>
       <c r="D98" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E98" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>201</v>
+        <v>71</v>
       </c>
       <c r="B99">
         <v>4</v>
@@ -2564,15 +2738,15 @@
         <v>4.5</v>
       </c>
       <c r="D99" t="s">
-        <v>202</v>
+        <v>72</v>
       </c>
       <c r="E99" t="s">
-        <v>154</v>
+        <v>35</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>203</v>
+        <v>73</v>
       </c>
       <c r="B100">
         <v>4</v>
@@ -2581,15 +2755,15 @@
         <v>3</v>
       </c>
       <c r="D100" t="s">
-        <v>204</v>
+        <v>74</v>
       </c>
       <c r="E100" t="s">
-        <v>134</v>
+        <v>33</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>205</v>
+        <v>75</v>
       </c>
       <c r="B101">
         <v>2</v>
@@ -2598,10 +2772,10 @@
         <v>1</v>
       </c>
       <c r="D101" t="s">
-        <v>206</v>
+        <v>76</v>
       </c>
       <c r="E101" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>